<commit_message>
Added error log to excel
</commit_message>
<xml_diff>
--- a/reg.xlsx
+++ b/reg.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="ошибки" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Менеджер</t>
   </si>
@@ -34,23 +35,46 @@
     <t>Текст заявки</t>
   </si>
   <si>
-    <t>Алексей Мельхер</t>
-  </si>
-  <si>
-    <t>доставка</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ООО «М Бетон» </t>
-  </si>
-  <si>
-    <t>\nАлексей Мельхер:\nЗаявка на доставку \n1.Дата отгрузки 28.04\n2. Марка: ЦЕМ I 42.5Н Костюковичи \n3. Количество тонн: 70     \n4. Продажа от ООО "СЗТК" \n5. С Солнечногорска \n6. Покупатель ООО «М Бетон» \n7. Грузополучатель ООО «М-Бетон» \n8. Юр.Адрес грузополучателя: 109382, г. Москва, вн. тер. г. муниципальный округ Люблино, ул. Люблинская, д. 72, помещ. 26 \n9. Пункт разгрузки: Москва г, Очаковское ш., дом 5А, въезд с проезда Стройкомбината\n10. Контакты для связи 8-925-758-01-54\n</t>
+    <t>\nИГО:\nЗаявка на доставку \n1. Дата отгрузки 28.04.2023 \n2. Марка ЦЕМ I 42.5н Беларусь   \n3. Количество тонн: 100 \n4. От ООО Спарта \n5. Завод: Сзтк \n6. Покупатель ООО ""ТД"Цемент \n7. Грузополучатель: ООО "ТД"Цемент  \n8. Голицыно\n+7 910 404-06-14\nРБУ\nМожайское ш., 81\n</t>
+  </si>
+  <si>
+    <t>Ошибка</t>
+  </si>
+  <si>
+    <t>Заявка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Traceback (most recent call last):
+  File "C:\Users\79852\Desktop\gh\applications\applic.py", line 64, in find_unit_note
+    unit_found = self.units_df.loc[self.units_df[self.units_df['data'] == unit].index[0], 'unit']
+  File "C:\Users\79852\anaconda3\lib\site-packages\pandas\core\indexes\base.py", line 5039, in __getitem__
+    return getitem(key)
+IndexError: index 0 is out of bounds for axis 0 with size 0
+During handling of the above exception, another exception occurred:
+Traceback (most recent call last):
+  File "C:\Users\79852\Desktop\gh\applications\applic.py", line 91, in process_application
+    unit_found = self.find_unit_note(application)
+  File "C:\Users\79852\Desktop\gh\applications\applic.py", line 67, in find_unit_note
+    self.error_log.append(f"Ошибка в методе find_unit_note: {e}")
+  File "C:\Users\79852\anaconda3\lib\site-packages\pandas\core\frame.py", line 9039, in append
+    return self._append(other, ignore_index, verify_integrity, sort)
+  File "C:\Users\79852\anaconda3\lib\site-packages\pandas\core\frame.py", line 9082, in _append
+    result = concat(
+  File "C:\Users\79852\anaconda3\lib\site-packages\pandas\util\_decorators.py", line 311, in wrapper
+    return func(*args, **kwargs)
+  File "C:\Users\79852\anaconda3\lib\site-packages\pandas\core\reshape\concat.py", line 347, in concat
+    op = _Concatenator(
+  File "C:\Users\79852\anaconda3\lib\site-packages\pandas\core\reshape\concat.py", line 437, in __init__
+    raise TypeError(msg)
+TypeError: cannot concatenate object of type '&lt;class 'str'&gt;'; only Series and DataFrame objs are valid
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,24 +126,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -157,7 +189,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -191,6 +223,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -225,9 +258,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -400,14 +434,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -427,21 +461,43 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="47.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="96.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2">
-        <v>70</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>